<commit_message>
Add Input field wtih to enter location, added validation Add Refresh button to reload table if input field is valid
</commit_message>
<xml_diff>
--- a/WialonApp/wwwroot/WeatherData.xlsx
+++ b/WialonApp/wwwroot/WeatherData.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Weather Data" sheetId="1" r:id="R66b96f4f81d64a59"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Weather Data" sheetId="1" r:id="Rd1b3607875994ac7"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -65,7 +65,7 @@
         <x:v>Location</x:v>
       </x:c>
       <x:c s="3" t="str">
-        <x:v>Pleven</x:v>
+        <x:v>Sofia</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -73,7 +73,7 @@
         <x:v>Latitude</x:v>
       </x:c>
       <x:c s="0" t="str">
-        <x:v>43.4167</x:v>
+        <x:v>42.6975</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -81,7 +81,7 @@
         <x:v>Longitude</x:v>
       </x:c>
       <x:c s="3" t="str">
-        <x:v>24.6167</x:v>
+        <x:v>23.3242</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -89,7 +89,7 @@
         <x:v>Condition</x:v>
       </x:c>
       <x:c s="0" t="str">
-        <x:v>Clouds</x:v>
+        <x:v>Clear</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -97,7 +97,7 @@
         <x:v>Description</x:v>
       </x:c>
       <x:c s="3" t="str">
-        <x:v>few clouds</x:v>
+        <x:v>clear sky</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -105,7 +105,7 @@
         <x:v>Temperature</x:v>
       </x:c>
       <x:c s="0" t="str">
-        <x:v>2.97 °C (Feels like 2.97 °C)</x:v>
+        <x:v>7.83 °C (Feels like 7.83 °C)</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -113,7 +113,7 @@
         <x:v>Temperature Range</x:v>
       </x:c>
       <x:c s="3" t="str">
-        <x:v>2.97 °C to 9.33 °C</x:v>
+        <x:v>7.83 °C to 7.83 °C</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -121,7 +121,7 @@
         <x:v>Pressure</x:v>
       </x:c>
       <x:c s="0" t="str">
-        <x:v>1034 hPa</x:v>
+        <x:v>1032 hPa</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -129,7 +129,7 @@
         <x:v>Humidity</x:v>
       </x:c>
       <x:c s="3" t="str">
-        <x:v>65%</x:v>
+        <x:v>42%</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -137,7 +137,7 @@
         <x:v>Wind</x:v>
       </x:c>
       <x:c s="0" t="str">
-        <x:v>1.03 m/s at 180°</x:v>
+        <x:v>1.03 m/s at 0°</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -145,7 +145,7 @@
         <x:v>Cloudiness</x:v>
       </x:c>
       <x:c s="3" t="str">
-        <x:v>20%</x:v>
+        <x:v>0%</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -161,7 +161,7 @@
         <x:v>Sunrise</x:v>
       </x:c>
       <x:c s="3" t="str">
-        <x:v>06:03</x:v>
+        <x:v>06:07</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -169,7 +169,7 @@
         <x:v>Sunset</x:v>
       </x:c>
       <x:c s="0" t="str">
-        <x:v>16:06</x:v>
+        <x:v>16:13</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Add Tests Minor fixes
</commit_message>
<xml_diff>
--- a/WialonApp/wwwroot/WeatherData.xlsx
+++ b/WialonApp/wwwroot/WeatherData.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Weather Data" sheetId="1" r:id="Rd1b3607875994ac7"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Weather Data" sheetId="1" r:id="Rf89cd596518a487d"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -105,7 +105,7 @@
         <x:v>Temperature</x:v>
       </x:c>
       <x:c s="0" t="str">
-        <x:v>7.83 °C (Feels like 7.83 °C)</x:v>
+        <x:v>12.55 °C (Feels like 10.88 °C)</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -113,7 +113,7 @@
         <x:v>Temperature Range</x:v>
       </x:c>
       <x:c s="3" t="str">
-        <x:v>7.83 °C to 7.83 °C</x:v>
+        <x:v>12.32 °C to 13.91 °C</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -121,7 +121,7 @@
         <x:v>Pressure</x:v>
       </x:c>
       <x:c s="0" t="str">
-        <x:v>1032 hPa</x:v>
+        <x:v>1030 hPa</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -129,7 +129,7 @@
         <x:v>Humidity</x:v>
       </x:c>
       <x:c s="3" t="str">
-        <x:v>42%</x:v>
+        <x:v>39%</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -137,7 +137,7 @@
         <x:v>Wind</x:v>
       </x:c>
       <x:c s="0" t="str">
-        <x:v>1.03 m/s at 0°</x:v>
+        <x:v>1.54 m/s at 140°</x:v>
       </x:c>
     </x:row>
     <x:row>

</xml_diff>